<commit_message>
cambio tabla 1 de los datos raw
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97577F23-C057-42F4-B163-FE07A8E84DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23538FF-DF85-415B-ABE5-6FA5579E08AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6158" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6160" uniqueCount="1021">
   <si>
     <t>Health Index Asset Category</t>
   </si>
@@ -3405,6 +3405,9 @@
   </si>
   <si>
     <t>132kV Trabsformer (GM)</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
   </si>
 </sst>
 </file>
@@ -3505,7 +3508,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3516,6 +3519,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3531,7 +3540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3582,6 +3591,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3668,9 +3678,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3708,7 +3718,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3814,7 +3824,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3956,7 +3966,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3964,10 +3974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,6 +4481,14 @@
       </c>
       <c r="B62" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="26" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -12650,14 +12668,15 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
@@ -14342,17 +14361,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
@@ -18051,7 +18070,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="79.7109375" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
     <col min="5" max="1025" width="8.85546875" customWidth="1"/>

</xml_diff>